<commit_message>
chore: modify graph line length
</commit_message>
<xml_diff>
--- a/assets/鋼筋型文對照表-20230426_鋼筋計料.xlsx
+++ b/assets/鋼筋型文對照表-20230426_鋼筋計料.xlsx
@@ -857,8 +857,8 @@
       </c>
       <c r="H12" s="5" t="inlineStr">
         <is>
-          <t>150
-───</t>
+          <t xml:space="preserve">   150
+──────────</t>
         </is>
       </c>
       <c r="I12" s="5" t="inlineStr">
@@ -893,8 +893,8 @@
       </c>
       <c r="H13" s="5" t="inlineStr">
         <is>
-          <t>150
-───</t>
+          <t xml:space="preserve">   150
+──────────</t>
         </is>
       </c>
       <c r="I13" s="5" t="inlineStr">
@@ -929,8 +929,8 @@
       </c>
       <c r="H14" s="5" t="inlineStr">
         <is>
-          <t>150
-───</t>
+          <t xml:space="preserve">   150
+──────────</t>
         </is>
       </c>
       <c r="I14" s="5" t="inlineStr">
@@ -965,8 +965,8 @@
       </c>
       <c r="H15" s="5" t="inlineStr">
         <is>
-          <t>50
-───</t>
+          <t xml:space="preserve">    50
+──────────</t>
         </is>
       </c>
       <c r="I15" s="5" t="inlineStr">
@@ -1002,7 +1002,7 @@
       <c r="H16" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">   495
-─────────</t>
+──────────</t>
         </is>
       </c>
       <c r="I16" s="5" t="inlineStr">
@@ -1037,8 +1037,8 @@
       </c>
       <c r="H17" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    200      
-20 |────| 200</t>
+          <t xml:space="preserve">       200         
+20 |──────────| 200</t>
         </is>
       </c>
       <c r="I17" s="5" t="inlineStr">
@@ -1073,8 +1073,8 @@
       </c>
       <c r="H18" s="5" t="inlineStr">
         <is>
-          <t>200
-────</t>
+          <t xml:space="preserve">   200
+──────────</t>
         </is>
       </c>
       <c r="I18" s="5" t="inlineStr">
@@ -1109,8 +1109,8 @@
       </c>
       <c r="H19" s="5" t="inlineStr">
         <is>
-          <t>40
-───</t>
+          <t xml:space="preserve">    40
+──────────</t>
         </is>
       </c>
       <c r="I19" s="5" t="inlineStr">
@@ -1145,8 +1145,8 @@
       </c>
       <c r="H20" s="5" t="inlineStr">
         <is>
-          <t>41
-───</t>
+          <t xml:space="preserve">    41
+──────────</t>
         </is>
       </c>
       <c r="I20" s="5" t="inlineStr">
@@ -1181,8 +1181,8 @@
       </c>
       <c r="H21" s="5" t="inlineStr">
         <is>
-          <t>41
-───</t>
+          <t xml:space="preserve">    41
+──────────</t>
         </is>
       </c>
       <c r="I21" s="5" t="inlineStr">
@@ -1217,8 +1217,8 @@
       </c>
       <c r="H22" s="5" t="inlineStr">
         <is>
-          <t>41
-───</t>
+          <t xml:space="preserve">    41
+──────────</t>
         </is>
       </c>
       <c r="I22" s="5" t="inlineStr">
@@ -1289,8 +1289,8 @@
       </c>
       <c r="H24" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    200     
-25 |────| 25</t>
+          <t xml:space="preserve">       200        
+25 |──────────| 25</t>
         </is>
       </c>
       <c r="I24" s="5" t="inlineStr">
@@ -1325,8 +1325,8 @@
       </c>
       <c r="H25" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    200     
-25 |────| 25</t>
+          <t xml:space="preserve">       200        
+25 |──────────| 25</t>
         </is>
       </c>
       <c r="I25" s="5" t="inlineStr">
@@ -1361,8 +1361,8 @@
       </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    200     
-25 |────| 50</t>
+          <t xml:space="preserve">       200        
+25 |──────────| 50</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr">
@@ -1397,8 +1397,8 @@
       </c>
       <c r="H27" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    200     
-25 |────| 25</t>
+          <t xml:space="preserve">       200        
+25 |──────────| 25</t>
         </is>
       </c>
       <c r="I27" s="5" t="inlineStr">
@@ -1434,7 +1434,7 @@
       <c r="H28" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">   450
-─────────</t>
+──────────</t>
         </is>
       </c>
       <c r="I28" s="5" t="inlineStr">
@@ -1469,8 +1469,8 @@
       </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">       450        
-20 |─────────| 450</t>
+          <t xml:space="preserve">       450         
+20 |──────────| 450</t>
         </is>
       </c>
       <c r="I29" s="5" t="inlineStr">
@@ -1505,8 +1505,8 @@
       </c>
       <c r="H30" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">     100     
-100 |───| 100</t>
+          <t xml:space="preserve">        100         
+100 |──────────| 100</t>
         </is>
       </c>
       <c r="I30" s="5" t="inlineStr">
@@ -1541,8 +1541,8 @@
       </c>
       <c r="H31" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">     300      
-50 |──────| 50</t>
+          <t xml:space="preserve">       300        
+50 |──────────| 50</t>
         </is>
       </c>
       <c r="I31" s="5" t="inlineStr">
@@ -1577,8 +1577,8 @@
       </c>
       <c r="H32" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">     300      
-50 |──────| 50</t>
+          <t xml:space="preserve">       300        
+50 |──────────| 50</t>
         </is>
       </c>
       <c r="I32" s="5" t="inlineStr">

</xml_diff>

<commit_message>
feat: modify ui styles
</commit_message>
<xml_diff>
--- a/assets/鋼筋型文對照表-20230426_鋼筋計料.xlsx
+++ b/assets/鋼筋型文對照表-20230426_鋼筋計料.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="鋼筋計料" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="鋼筋計料表" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,8 +39,11 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -55,8 +58,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FFF2E7"/>
+        <bgColor rgb="00FFF2E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7F3FF"/>
+        <bgColor rgb="00E7F3FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00E2EFDA"/>
         <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F3E7FF"/>
+        <bgColor rgb="00F3E7FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -84,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -104,12 +125,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -475,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,21 +514,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="60" customWidth="1" min="8" max="8"/>
-    <col width="60" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="80" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>鋼筋計料表</t>
+          <t>🏗️ 專業鋼筋計料表 （含專業圖形化圖示）</t>
         </is>
       </c>
     </row>
@@ -511,94 +543,70 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>生成時間: 2025-06-03 11:41:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+          <t>生成時間: 2025-06-03 16:18:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>工具版本: CAD 鋼筋計料轉換工具 Pro v2.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>編號</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>長度(cm)</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C6" s="4" t="inlineStr">
         <is>
           <t>A(cm)</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D6" s="4" t="inlineStr">
         <is>
           <t>B(cm)</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="E6" s="4" t="inlineStr">
         <is>
           <t>C(cm)</t>
         </is>
       </c>
-      <c r="F5" s="4" t="inlineStr">
+      <c r="F6" s="4" t="inlineStr">
         <is>
           <t>數量</t>
         </is>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="G6" s="4" t="inlineStr">
         <is>
           <t>總重量(kg)</t>
         </is>
       </c>
-      <c r="H5" s="4" t="inlineStr">
-        <is>
-          <t>圖示</t>
-        </is>
-      </c>
-      <c r="I5" s="4" t="inlineStr">
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>材料等級</t>
+        </is>
+      </c>
+      <c r="I6" s="4" t="inlineStr">
+        <is>
+          <t>鋼筋圖示</t>
+        </is>
+      </c>
+      <c r="J6" s="4" t="inlineStr">
         <is>
           <t>備註</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="60" customHeight="1">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>#10</t>
-        </is>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>500</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>500</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="n">
-        <v>320.2</v>
-      </c>
-      <c r="H6" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   500
-──────────</t>
-        </is>
-      </c>
-      <c r="I6" s="6" t="inlineStr">
-        <is>
-          <t>公#10-500x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="60" customHeight="1">
+    <row r="7" ht="120" customHeight="1">
       <c r="A7" s="5" t="inlineStr">
         <is>
           <t>#10</t>
@@ -622,55 +630,73 @@
       <c r="G7" s="6" t="n">
         <v>320.2</v>
       </c>
-      <c r="H7" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   500
-──────────</t>
+      <c r="H7" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
         </is>
       </c>
       <c r="I7" s="6" t="inlineStr">
         <is>
+          <t>直鋼筋 #10
+長度: 500cm
+等級: SD420
+├───────────┤
+  500cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J7" s="6" t="inlineStr">
+        <is>
+          <t>公#10-500x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="120" customHeight="1">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>#10</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>320.2</v>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
+        </is>
+      </c>
+      <c r="I8" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #10
+長度: 500cm
+等級: SD420
+├───────────┤
+  500cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J8" s="6" t="inlineStr">
+        <is>
           <t>母#10-500x10</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="60" customHeight="1">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>#10</t>
-        </is>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>700</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>448.28</v>
-      </c>
-      <c r="H8" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   700
-──────────</t>
-        </is>
-      </c>
-      <c r="I8" s="6" t="inlineStr">
-        <is>
-          <t>公公#10-700x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="60" customHeight="1">
+    <row r="9" ht="120" customHeight="1">
       <c r="A9" s="5" t="inlineStr">
         <is>
           <t>#10</t>
@@ -694,55 +720,73 @@
       <c r="G9" s="6" t="n">
         <v>448.28</v>
       </c>
-      <c r="H9" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   700
-──────────</t>
+      <c r="H9" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
         </is>
       </c>
       <c r="I9" s="6" t="inlineStr">
         <is>
+          <t>直鋼筋 #10
+長度: 700cm
+等級: SD420
+├───────────┤
+  700cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J9" s="6" t="inlineStr">
+        <is>
+          <t>公公#10-700x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="120" customHeight="1">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>#10</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>700</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>448.28</v>
+      </c>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #10
+長度: 700cm
+等級: SD420
+├───────────┤
+  700cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J10" s="6" t="inlineStr">
+        <is>
           <t>母母#10-700x10</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>#10</t>
-        </is>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>805</v>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>750</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>515.52</v>
-      </c>
-      <c r="H10" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       750         
-55 |──────────| 750</t>
-        </is>
-      </c>
-      <c r="I10" s="6" t="inlineStr">
-        <is>
-          <t>公#10-55+750x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="60" customHeight="1">
+    <row r="11" ht="120" customHeight="1">
       <c r="A11" s="5" t="inlineStr">
         <is>
           <t>#10</t>
@@ -766,55 +810,83 @@
       <c r="G11" s="6" t="n">
         <v>515.52</v>
       </c>
-      <c r="H11" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       750         
-55 |──────────| 750</t>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
         </is>
       </c>
       <c r="I11" s="6" t="inlineStr">
         <is>
+          <t>L型鋼筋 #10
+等級: SD420
+彎曲半徑: R10cm
+    55cm
+┌──────────┐
+│          │
+│          │
+│          │ 750cm
+│          │
+│          │
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J11" s="6" t="inlineStr">
+        <is>
+          <t>公#10-55+750x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="120" customHeight="1">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>#10</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>805</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>750</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>515.52</v>
+      </c>
+      <c r="H12" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
+        </is>
+      </c>
+      <c r="I12" s="6" t="inlineStr">
+        <is>
+          <t>L型鋼筋 #10
+等級: SD420
+彎曲半徑: R10cm
+    55cm
+┌──────────┐
+│          │
+│          │
+│          │ 750cm
+│          │
+│          │
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J12" s="6" t="inlineStr">
+        <is>
           <t>母#10-55+750x10</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>#10</t>
-        </is>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>500</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>500</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E12" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F12" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6" t="n">
-        <v>320.2</v>
-      </c>
-      <c r="H12" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   500
-──────────</t>
-        </is>
-      </c>
-      <c r="I12" s="6" t="inlineStr">
-        <is>
-          <t>T#10-500x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="60" customHeight="1">
+    <row r="13" ht="120" customHeight="1">
       <c r="A13" s="5" t="inlineStr">
         <is>
           <t>#10</t>
@@ -838,55 +910,73 @@
       <c r="G13" s="6" t="n">
         <v>320.2</v>
       </c>
-      <c r="H13" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   500
-──────────</t>
+      <c r="H13" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
         </is>
       </c>
       <c r="I13" s="6" t="inlineStr">
         <is>
+          <t>直鋼筋 #10
+長度: 500cm
+等級: SD420
+├───────────┤
+  500cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J13" s="6" t="inlineStr">
+        <is>
+          <t>T#10-500x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="120" customHeight="1">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>#10</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>320.2</v>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
+        </is>
+      </c>
+      <c r="I14" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #10
+長度: 500cm
+等級: SD420
+├───────────┤
+  500cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J14" s="6" t="inlineStr">
+        <is>
           <t>公母#10-500x10</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="60" customHeight="1">
-      <c r="A14" s="5" t="inlineStr">
-        <is>
-          <t>#3</t>
-        </is>
-      </c>
-      <c r="B14" s="6" t="n">
-        <v>150</v>
-      </c>
-      <c r="C14" s="6" t="n">
-        <v>150</v>
-      </c>
-      <c r="D14" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E14" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F14" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6" t="n">
-        <v>8.42</v>
-      </c>
-      <c r="H14" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   150
-──────────</t>
-        </is>
-      </c>
-      <c r="I14" s="6" t="inlineStr">
-        <is>
-          <t>（例: #3-150x10*10 ← 總數100隻）</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="60" customHeight="1">
+    <row r="15" ht="120" customHeight="1">
       <c r="A15" s="5" t="inlineStr">
         <is>
           <t>#3</t>
@@ -910,19 +1000,28 @@
       <c r="G15" s="6" t="n">
         <v>8.42</v>
       </c>
-      <c r="H15" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   150
-──────────</t>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I15" s="6" t="inlineStr">
         <is>
-          <t>（例: #3-150x10隻）</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="60" customHeight="1">
+          <t>直鋼筋 #3
+長度: 150cm
+等級: SD280
+├───────────┤
+  150cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J15" s="6" t="inlineStr">
+        <is>
+          <t>（例: #3-150x10*10 ← 總數100隻）</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="120" customHeight="1">
       <c r="A16" s="5" t="inlineStr">
         <is>
           <t>#3</t>
@@ -946,235 +1045,303 @@
       <c r="G16" s="6" t="n">
         <v>8.42</v>
       </c>
-      <c r="H16" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   150
-──────────</t>
+      <c r="H16" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I16" s="6" t="inlineStr">
         <is>
+          <t>直鋼筋 #3
+長度: 150cm
+等級: SD280
+├───────────┤
+  150cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J16" s="6" t="inlineStr">
+        <is>
+          <t>（例: #3-150x10隻）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="120" customHeight="1">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>#3</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>8.42</v>
+      </c>
+      <c r="H17" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I17" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #3
+長度: 150cm
+等級: SD280
+├───────────┤
+  150cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J17" s="6" t="inlineStr">
+        <is>
           <t>#3-150x10</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="60" customHeight="1">
-      <c r="A17" s="5" t="inlineStr">
+    <row r="18" ht="120" customHeight="1">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>#3</t>
         </is>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B18" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C18" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="D17" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E17" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F17" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G17" s="6" t="n">
+      <c r="D18" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6" t="n">
         <v>2.81</v>
       </c>
-      <c r="H17" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    50
-──────────</t>
-        </is>
-      </c>
-      <c r="I17" s="6" t="inlineStr">
+      <c r="H18" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I18" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #3
+長度: 50cm
+等級: SD280
+├──────────┤
+  50cm
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J18" s="6" t="inlineStr">
         <is>
           <t>帽蓋#3-50x10</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="60" customHeight="1">
-      <c r="A18" s="5" t="inlineStr">
+    <row r="19" ht="120" customHeight="1">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B19" s="6" t="n">
         <v>495</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C19" s="6" t="n">
         <v>495</v>
       </c>
-      <c r="D18" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F18" s="6" t="n">
+      <c r="D19" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F19" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G18" s="6" t="n">
+      <c r="G19" s="6" t="n">
         <v>4.93</v>
       </c>
-      <c r="H18" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   495
-──────────</t>
-        </is>
-      </c>
-      <c r="I18" s="6" t="inlineStr">
+      <c r="H19" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I19" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #4
+長度: 495cm
+等級: SD280
+├───────────┤
+  495cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J19" s="6" t="inlineStr">
         <is>
           <t>（例: 異型箍    總長495，則以單T頭料 "T#4-495x1" 去計，以長度數量正確為原則，最後輸出料單後改圖示即可）</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="60" customHeight="1">
-      <c r="A19" s="5" t="inlineStr">
+    <row r="20" ht="120" customHeight="1">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B20" s="6" t="n">
         <v>220</v>
       </c>
-      <c r="C19" s="6" t="n">
+      <c r="C20" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D19" s="6" t="n">
+      <c r="D20" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="E19" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G19" s="6" t="n">
+      <c r="E20" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G20" s="6" t="n">
         <v>21.91</v>
       </c>
-      <c r="H19" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       200         
-20 |──────────| 200</t>
-        </is>
-      </c>
-      <c r="I19" s="6" t="inlineStr">
+      <c r="H20" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I20" s="6" t="inlineStr">
+        <is>
+          <t>L型鋼筋 #4
+等級: SD280
+彎曲半徑: R4cm
+    20cm
+┌──────────┐
+│          │
+│          │
+│          │ 200cm
+│          │
+│          │
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J20" s="6" t="inlineStr">
         <is>
           <t>#4-20+200x10</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="60" customHeight="1">
-      <c r="A20" s="5" t="inlineStr">
+    <row r="21" ht="120" customHeight="1">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B21" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C21" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="D20" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E20" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F20" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G20" s="6" t="n">
+      <c r="D21" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G21" s="6" t="n">
         <v>19.92</v>
       </c>
-      <c r="H20" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   200
-──────────</t>
-        </is>
-      </c>
-      <c r="I20" s="6" t="inlineStr">
+      <c r="H21" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I21" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #4
+長度: 200cm
+等級: SD280
+├───────────┤
+  200cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J21" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">#4-200x10  </t>
         </is>
       </c>
     </row>
-    <row r="21" ht="60" customHeight="1">
-      <c r="A21" s="5" t="inlineStr">
+    <row r="22" ht="120" customHeight="1">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B22" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="C21" s="6" t="n">
+      <c r="C22" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="D21" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F21" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G21" s="6" t="n">
+      <c r="D22" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G22" s="6" t="n">
         <v>3.98</v>
       </c>
-      <c r="H21" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    40
-──────────</t>
-        </is>
-      </c>
-      <c r="I21" s="6" t="inlineStr">
+      <c r="H22" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I22" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #4
+長度: 40cm
+等級: SD280
+├──────────┤
+  40cm
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J22" s="6" t="inlineStr">
         <is>
           <t>梁繫#4-40x10</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="60" customHeight="1">
-      <c r="A22" s="5" t="inlineStr">
-        <is>
-          <t>#4</t>
-        </is>
-      </c>
-      <c r="B22" s="6" t="n">
-        <v>41</v>
-      </c>
-      <c r="C22" s="6" t="n">
-        <v>41</v>
-      </c>
-      <c r="D22" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E22" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F22" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G22" s="6" t="n">
-        <v>4.08</v>
-      </c>
-      <c r="H22" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    41
-──────────</t>
-        </is>
-      </c>
-      <c r="I22" s="6" t="inlineStr">
-        <is>
-          <t>柱繫#4-41x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="60" customHeight="1">
+    <row r="23" ht="120" customHeight="1">
       <c r="A23" s="5" t="inlineStr">
         <is>
           <t>#4</t>
@@ -1198,19 +1365,28 @@
       <c r="G23" s="6" t="n">
         <v>4.08</v>
       </c>
-      <c r="H23" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    41
-──────────</t>
+      <c r="H23" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I23" s="6" t="inlineStr">
         <is>
-          <t>牆繫#4-41x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="60" customHeight="1">
+          <t>直鋼筋 #4
+長度: 41cm
+等級: SD280
+├──────────┤
+  41cm
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J23" s="6" t="inlineStr">
+        <is>
+          <t>柱繫#4-41x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="120" customHeight="1">
       <c r="A24" s="5" t="inlineStr">
         <is>
           <t>#4</t>
@@ -1234,91 +1410,118 @@
       <c r="G24" s="6" t="n">
         <v>4.08</v>
       </c>
-      <c r="H24" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    41
-──────────</t>
+      <c r="H24" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I24" s="6" t="inlineStr">
         <is>
+          <t>直鋼筋 #4
+長度: 41cm
+等級: SD280
+├──────────┤
+  41cm
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J24" s="6" t="inlineStr">
+        <is>
+          <t>牆繫#4-41x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="120" customHeight="1">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>#4</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="C25" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="D25" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E25" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F25" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="H25" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I25" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #4
+長度: 41cm
+等級: SD280
+├──────────┤
+  41cm
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J25" s="6" t="inlineStr">
+        <is>
           <t>樑柱繫#4-41x10</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="60" customHeight="1">
-      <c r="A25" s="5" t="inlineStr">
+    <row r="26" ht="120" customHeight="1">
+      <c r="A26" s="5" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="B25" s="6" t="n">
+      <c r="B26" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="C25" s="6" t="n">
+      <c r="C26" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="D25" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E25" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F25" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G25" s="6" t="n">
+      <c r="D26" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E26" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F26" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G26" s="6" t="n">
         <v>49.8</v>
       </c>
-      <c r="H25" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   500
-──────────</t>
-        </is>
-      </c>
-      <c r="I25" s="6" t="inlineStr">
+      <c r="H26" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I26" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #4
+長度: 500cm
+等級: SD280
+├───────────┤
+  500cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J26" s="6" t="inlineStr">
         <is>
           <t>弧300#4-500x10</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="60" customHeight="1">
-      <c r="A26" s="5" t="inlineStr">
-        <is>
-          <t>#5</t>
-        </is>
-      </c>
-      <c r="B26" s="6" t="n">
-        <v>250</v>
-      </c>
-      <c r="C26" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D26" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="E26" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G26" s="6" t="n">
-        <v>38.8</v>
-      </c>
-      <c r="H26" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       200        
-25 |──────────| 25</t>
-        </is>
-      </c>
-      <c r="I26" s="6" t="inlineStr">
-        <is>
-          <t>#5-25+200+25x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="60" customHeight="1">
+    <row r="27" ht="120" customHeight="1">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>#5</t>
@@ -1342,26 +1545,38 @@
       <c r="G27" s="6" t="n">
         <v>38.8</v>
       </c>
-      <c r="H27" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       200        
-25 |──────────| 25</t>
+      <c r="H27" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I27" s="6" t="inlineStr">
         <is>
-          <t>寬止#5-25+200+25x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="60" customHeight="1">
+          <t>U型鋼筋 #5
+等級: SD280
+彎曲半徑: R5cm
+200cm     25cm     25cm
+│                │
+│                │
+│                │
+│                │
+└────────────────┘</t>
+        </is>
+      </c>
+      <c r="J27" s="6" t="inlineStr">
+        <is>
+          <t>#5-25+200+25x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="120" customHeight="1">
       <c r="A28" s="5" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
       <c r="B28" s="6" t="n">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>25</v>
@@ -1370,34 +1585,46 @@
         <v>200</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F28" s="6" t="n">
         <v>10</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>42.68</v>
-      </c>
-      <c r="H28" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       200        
-25 |──────────| 50</t>
+        <v>38.8</v>
+      </c>
+      <c r="H28" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I28" s="6" t="inlineStr">
         <is>
-          <t>#5-25+200+50x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="60" customHeight="1">
+          <t>U型鋼筋 #5
+等級: SD280
+彎曲半徑: R5cm
+200cm     25cm     25cm
+│                │
+│                │
+│                │
+│                │
+└────────────────┘</t>
+        </is>
+      </c>
+      <c r="J28" s="6" t="inlineStr">
+        <is>
+          <t>寬止#5-25+200+25x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="120" customHeight="1">
       <c r="A29" s="5" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
       <c r="B29" s="6" t="n">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>25</v>
@@ -1406,171 +1633,232 @@
         <v>200</v>
       </c>
       <c r="E29" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>42.68</v>
+      </c>
+      <c r="H29" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I29" s="6" t="inlineStr">
+        <is>
+          <t>U型鋼筋 #5
+等級: SD280
+彎曲半徑: R5cm
+200cm     25cm     50cm
+│                │
+│                │
+│                │
+│                │
+└────────────────┘</t>
+        </is>
+      </c>
+      <c r="J29" s="6" t="inlineStr">
+        <is>
+          <t>#5-25+200+50x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="120" customHeight="1">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>250</v>
+      </c>
+      <c r="C30" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="F29" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G29" s="6" t="n">
+      <c r="D30" s="6" t="n">
+        <v>200</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G30" s="6" t="n">
         <v>38.8</v>
       </c>
-      <c r="H29" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       200        
-25 |──────────| 25</t>
-        </is>
-      </c>
-      <c r="I29" s="6" t="inlineStr">
+      <c r="H30" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I30" s="6" t="inlineStr">
+        <is>
+          <t>U型鋼筋 #5
+等級: SD280
+彎曲半徑: R5cm
+200cm     25cm     25cm
+│                │
+│                │
+│                │
+│                │
+└────────────────┘</t>
+        </is>
+      </c>
+      <c r="J30" s="6" t="inlineStr">
         <is>
           <t>文武#5-25+200+25x10</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="60" customHeight="1">
-      <c r="A30" s="5" t="inlineStr">
+    <row r="31" ht="120" customHeight="1">
+      <c r="A31" s="5" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
-      <c r="B30" s="6" t="n">
+      <c r="B31" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="C30" s="6" t="n">
+      <c r="C31" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="D30" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E30" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F30" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G30" s="6" t="n">
+      <c r="D31" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E31" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G31" s="6" t="n">
         <v>69.84</v>
       </c>
-      <c r="H30" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   450
-──────────</t>
-        </is>
-      </c>
-      <c r="I30" s="6" t="inlineStr">
+      <c r="H31" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I31" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #5
+長度: 450cm
+等級: SD280
+├───────────┤
+  450cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J31" s="6" t="inlineStr">
         <is>
           <t>安#5-450x10</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="60" customHeight="1">
-      <c r="A31" s="5" t="inlineStr">
+    <row r="32" ht="120" customHeight="1">
+      <c r="A32" s="5" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
-      <c r="B31" s="6" t="n">
+      <c r="B32" s="6" t="n">
         <v>470</v>
       </c>
-      <c r="C31" s="6" t="n">
+      <c r="C32" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D32" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="E31" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F31" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G31" s="6" t="n">
+      <c r="E32" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G32" s="6" t="n">
         <v>72.94</v>
       </c>
-      <c r="H31" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       450         
-20 |──────────| 450</t>
-        </is>
-      </c>
-      <c r="I31" s="6" t="inlineStr">
+      <c r="H32" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I32" s="6" t="inlineStr">
+        <is>
+          <t>L型鋼筋 #5
+等級: SD280
+彎曲半徑: R5cm
+    20cm
+┌──────────┐
+│          │
+│          │
+│          │ 450cm
+│          │
+│          │
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J32" s="6" t="inlineStr">
         <is>
           <t>安#5-20+450x10</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="60" customHeight="1">
-      <c r="A32" s="5" t="inlineStr">
+    <row r="33" ht="120" customHeight="1">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>#6</t>
         </is>
       </c>
-      <c r="B32" s="6" t="n">
+      <c r="B33" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="C32" s="6" t="n">
+      <c r="C33" s="6" t="n">
         <v>100</v>
       </c>
-      <c r="D32" s="6" t="n">
+      <c r="D33" s="6" t="n">
         <v>100</v>
       </c>
-      <c r="E32" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F32" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G32" s="6" t="n">
+      <c r="E33" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F33" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G33" s="6" t="n">
         <v>44.7</v>
       </c>
-      <c r="H32" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        100         
-100 |──────────| 100</t>
-        </is>
-      </c>
-      <c r="I32" s="6" t="inlineStr">
+      <c r="H33" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I33" s="6" t="inlineStr">
+        <is>
+          <t>L型鋼筋 #6
+等級: SD280
+彎曲半徑: R6cm
+    100cm
+┌──────────┐
+│          │
+│          │
+│          │ 100cm
+│          │
+│          │
+└──────────┘</t>
+        </is>
+      </c>
+      <c r="J33" s="6" t="inlineStr">
         <is>
           <t>折135度#6-100+100x10</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="60" customHeight="1">
-      <c r="A33" s="5" t="inlineStr">
-        <is>
-          <t>#6</t>
-        </is>
-      </c>
-      <c r="B33" s="6" t="n">
-        <v>400</v>
-      </c>
-      <c r="C33" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="D33" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="E33" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F33" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G33" s="6" t="n">
-        <v>89.40000000000001</v>
-      </c>
-      <c r="H33" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       300        
-50 |──────────| 50</t>
-        </is>
-      </c>
-      <c r="I33" s="6" t="inlineStr">
-        <is>
-          <t>雙折#6-50+300+50x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="60" customHeight="1">
+    <row r="34" ht="120" customHeight="1">
       <c r="A34" s="5" t="inlineStr">
         <is>
           <t>#6</t>
@@ -1594,55 +1882,79 @@
       <c r="G34" s="6" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="H34" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">       300        
-50 |──────────| 50</t>
+      <c r="H34" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
         </is>
       </c>
       <c r="I34" s="6" t="inlineStr">
         <is>
+          <t>U型鋼筋 #6
+等級: SD280
+彎曲半徑: R6cm
+300cm     50cm     50cm
+│                │
+│                │
+│                │
+│                │
+└────────────────┘</t>
+        </is>
+      </c>
+      <c r="J34" s="6" t="inlineStr">
+        <is>
+          <t>雙折#6-50+300+50x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="120" customHeight="1">
+      <c r="A35" s="5" t="inlineStr">
+        <is>
+          <t>#6</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="C35" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>300</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <v>89.40000000000001</v>
+      </c>
+      <c r="H35" s="8" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="I35" s="6" t="inlineStr">
+        <is>
+          <t>U型鋼筋 #6
+等級: SD280
+彎曲半徑: R6cm
+300cm     50cm     50cm
+│                │
+│                │
+│                │
+│                │
+└────────────────┘</t>
+        </is>
+      </c>
+      <c r="J35" s="6" t="inlineStr">
+        <is>
           <t>雙折145度#6-50+300+50x10</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="60" customHeight="1">
-      <c r="A35" s="5" t="inlineStr">
-        <is>
-          <t>#8</t>
-        </is>
-      </c>
-      <c r="B35" s="6" t="n">
-        <v>650</v>
-      </c>
-      <c r="C35" s="6" t="n">
-        <v>650</v>
-      </c>
-      <c r="D35" s="6" t="n">
-        <v/>
-      </c>
-      <c r="E35" s="6" t="n">
-        <v/>
-      </c>
-      <c r="F35" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G35" s="6" t="n">
-        <v>258.25</v>
-      </c>
-      <c r="H35" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   650
-──────────</t>
-        </is>
-      </c>
-      <c r="I35" s="6" t="inlineStr">
-        <is>
-          <t>公母#8#7#6-650x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" ht="60" customHeight="1">
+    <row r="36" ht="120" customHeight="1">
       <c r="A36" s="5" t="inlineStr">
         <is>
           <t>#8</t>
@@ -1666,19 +1978,28 @@
       <c r="G36" s="6" t="n">
         <v>258.25</v>
       </c>
-      <c r="H36" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   650
-──────────</t>
+      <c r="H36" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
         </is>
       </c>
       <c r="I36" s="6" t="inlineStr">
         <is>
-          <t>公#8#7#6-650x10</t>
-        </is>
-      </c>
-    </row>
-    <row r="37" ht="60" customHeight="1">
+          <t>直鋼筋 #8
+長度: 650cm
+等級: SD420
+├───────────┤
+  650cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J36" s="6" t="inlineStr">
+        <is>
+          <t>公母#8#7#6-650x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="120" customHeight="1">
       <c r="A37" s="5" t="inlineStr">
         <is>
           <t>#8</t>
@@ -1702,39 +2023,153 @@
       <c r="G37" s="6" t="n">
         <v>258.25</v>
       </c>
-      <c r="H37" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   650
-──────────</t>
+      <c r="H37" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
         </is>
       </c>
       <c r="I37" s="6" t="inlineStr">
         <is>
+          <t>直鋼筋 #8
+長度: 650cm
+等級: SD420
+├───────────┤
+  650cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J37" s="6" t="inlineStr">
+        <is>
+          <t>公#8#7#6-650x10</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="120" customHeight="1">
+      <c r="A38" s="5" t="inlineStr">
+        <is>
+          <t>#8</t>
+        </is>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>650</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>650</v>
+      </c>
+      <c r="D38" s="6" t="n">
+        <v/>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v/>
+      </c>
+      <c r="F38" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G38" s="6" t="n">
+        <v>258.25</v>
+      </c>
+      <c r="H38" s="7" t="inlineStr">
+        <is>
+          <t>SD420</t>
+        </is>
+      </c>
+      <c r="I38" s="6" t="inlineStr">
+        <is>
+          <t>直鋼筋 #8
+長度: 650cm
+等級: SD420
+├───────────┤
+  650cm
+└───────────┘</t>
+        </is>
+      </c>
+      <c r="J38" s="6" t="inlineStr">
+        <is>
           <t>母#8#7#6-650x10</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="7" t="inlineStr">
+    <row r="40">
+      <c r="A40" s="9" t="inlineStr">
         <is>
           <t>總計</t>
         </is>
       </c>
-      <c r="B39" s="8" t="n"/>
-      <c r="C39" s="8" t="n"/>
-      <c r="D39" s="8" t="n"/>
-      <c r="E39" s="8" t="n"/>
-      <c r="F39" s="7" t="n">
+      <c r="B40" s="10" t="n"/>
+      <c r="C40" s="10" t="n"/>
+      <c r="D40" s="10" t="n"/>
+      <c r="E40" s="10" t="n"/>
+      <c r="F40" s="9" t="n">
         <v>311</v>
       </c>
-      <c r="G39" s="7" t="n">
+      <c r="G40" s="9" t="n">
         <v>4649.36</v>
       </c>
-      <c r="H39" s="8" t="n"/>
-      <c r="I39" s="8" t="n"/>
+      <c r="H40" s="10" t="n"/>
+      <c r="I40" s="10" t="n"/>
+      <c r="J40" s="10" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="11" t="inlineStr">
+        <is>
+          <t>材料等級說明:</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="12" t="inlineStr">
+        <is>
+          <t>SD280</t>
+        </is>
+      </c>
+      <c r="B44" s="12" t="inlineStr">
+        <is>
+          <t>280 MPa</t>
+        </is>
+      </c>
+      <c r="C44" s="12" t="inlineStr">
+        <is>
+          <t>一般結構用鋼筋</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="13" t="inlineStr">
+        <is>
+          <t>SD420</t>
+        </is>
+      </c>
+      <c r="B45" s="13" t="inlineStr">
+        <is>
+          <t>420 MPa</t>
+        </is>
+      </c>
+      <c r="C45" s="13" t="inlineStr">
+        <is>
+          <t>高強度結構鋼筋</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="14" t="inlineStr">
+        <is>
+          <t>SD490</t>
+        </is>
+      </c>
+      <c r="B46" s="14" t="inlineStr">
+        <is>
+          <t>490 MPa</t>
+        </is>
+      </c>
+      <c r="C46" s="14" t="inlineStr">
+        <is>
+          <t>特殊高強度鋼筋</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A4:H4"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A1:H1"/>

</xml_diff>